<commit_message>
"PlComponentCardPatient": corrected bugs in card_patient and card_status (hovering, male shape and female shape) + corrected contradictory names for status in 'database.xlsx' and 'pl_component_family_tree_viewer_d3_creator.css' (yet there are some status [e.g. 'muerte-subita', 'muerte-por-otras-causas'] that are not displayed correctly in *the family tree*.
</commit_message>
<xml_diff>
--- a/database/database.xlsx
+++ b/database/database.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26311"/>
-  <workbookPr showInkAnnotation="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlos/Documents/DevOps/patient_line/patient_line_viewer_family_tree/database/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="21405"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16920" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2420" yWindow="640" windowWidth="28800" windowHeight="16920" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Family" sheetId="1" r:id="rId1"/>
     <sheet name="general" sheetId="2" r:id="rId2"/>
     <sheet name="clinical values" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -175,12 +170,6 @@
     <t>sin-manifestacion-fenotipica</t>
   </si>
   <si>
-    <t>muerte-otras-causas</t>
-  </si>
-  <si>
-    <t>manifestacion-fenotipica</t>
-  </si>
-  <si>
     <t>diagnosed</t>
   </si>
   <si>
@@ -215,6 +204,12 @@
   </si>
   <si>
     <t>FJSL young brother</t>
+  </si>
+  <si>
+    <t>muerte-por-otras-causas</t>
+  </si>
+  <si>
+    <t>manifestacion-responsable</t>
   </si>
 </sst>
 </file>
@@ -310,7 +305,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -345,7 +340,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -522,7 +517,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -534,14 +529,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="24.6640625" customWidth="1"/>
     <col min="2" max="2" width="28.6640625" customWidth="1"/>
     <col min="3" max="3" width="82.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -552,7 +547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -563,7 +558,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -574,7 +569,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -587,6 +582,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -594,17 +594,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="6" max="6" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -630,7 +630,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -650,7 +650,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -670,7 +670,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -696,7 +696,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -716,12 +716,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
         <v>42</v>
@@ -739,7 +739,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -762,7 +762,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -785,7 +785,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -805,7 +805,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -825,7 +825,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -848,7 +848,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -873,6 +873,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -880,11 +885,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="4" max="4" width="23.33203125" customWidth="1"/>
     <col min="5" max="5" width="20.83203125" customWidth="1"/>
@@ -893,7 +898,7 @@
     <col min="8" max="8" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -919,10 +924,10 @@
         <v>23</v>
       </c>
       <c r="I1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -936,10 +941,10 @@
         <v>48</v>
       </c>
       <c r="I2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -950,13 +955,13 @@
         <v>47</v>
       </c>
       <c r="F3" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="I3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -964,22 +969,22 @@
         <v>25569</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" t="s">
         <v>50</v>
       </c>
-      <c r="G4" t="s">
-        <v>51</v>
-      </c>
-      <c r="H4" t="s">
-        <v>52</v>
-      </c>
       <c r="I4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -990,12 +995,12 @@
         <v>48</v>
       </c>
       <c r="I5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>61</v>
       </c>
       <c r="C6" s="1">
         <v>28856</v>
@@ -1007,10 +1012,10 @@
         <v>48</v>
       </c>
       <c r="I6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1024,15 +1029,15 @@
         <v>48</v>
       </c>
       <c r="I7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1043,10 +1048,10 @@
         <v>48</v>
       </c>
       <c r="I9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1057,10 +1062,10 @@
         <v>48</v>
       </c>
       <c r="I10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -1071,25 +1076,25 @@
         <v>34335</v>
       </c>
       <c r="D11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" t="s">
         <v>54</v>
       </c>
-      <c r="E11" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11" t="s">
-        <v>56</v>
-      </c>
       <c r="G11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -1100,25 +1105,30 @@
         <v>35796</v>
       </c>
       <c r="D12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E12" t="s">
         <v>47</v>
       </c>
       <c r="F12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" t="s">
+        <v>50</v>
+      </c>
+      <c r="I12" t="s">
         <v>57</v>
-      </c>
-      <c r="G12" t="s">
-        <v>51</v>
-      </c>
-      <c r="H12" t="s">
-        <v>52</v>
-      </c>
-      <c r="I12" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
refactor + PlPagePatients: done option to add a random family + when database is empty, added options of starting with a template database or creating a random family
</commit_message>
<xml_diff>
--- a/database/database.xlsx
+++ b/database/database.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="63">
   <si>
     <t>name</t>
   </si>
@@ -216,10 +216,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -242,14 +258,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -886,7 +906,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1036,6 +1056,9 @@
       <c r="A8" t="s">
         <v>44</v>
       </c>
+      <c r="F8" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
@@ -1125,6 +1148,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
- PlComponentSidebarFamily: now name and symptoms of a family are displayed at the top of the family tree viewer - PlComponentCardFamily: family's name, id, description and symptoms are editable
</commit_message>
<xml_diff>
--- a/database/database.xlsx
+++ b/database/database.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="64">
   <si>
     <t>name</t>
   </si>
@@ -210,6 +210,9 @@
   </si>
   <si>
     <t>manifestacion-responsable</t>
+  </si>
+  <si>
+    <t>comments</t>
   </si>
 </sst>
 </file>
@@ -537,7 +540,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -545,18 +548,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="24.6640625" customWidth="1"/>
     <col min="2" max="2" width="28.6640625" customWidth="1"/>
     <col min="3" max="3" width="82.6640625" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" customWidth="1"/>
+    <col min="5" max="5" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -566,8 +573,14 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -578,7 +591,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -589,7 +602,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -903,10 +916,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -916,9 +929,10 @@
     <col min="6" max="6" width="35.83203125" customWidth="1"/>
     <col min="7" max="7" width="15.5" customWidth="1"/>
     <col min="8" max="8" width="16.1640625" customWidth="1"/>
+    <col min="10" max="10" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -946,8 +960,11 @@
       <c r="I1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -964,7 +981,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -981,7 +998,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -1004,7 +1021,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -1018,7 +1035,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>59</v>
       </c>
@@ -1035,7 +1052,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1052,7 +1069,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -1060,7 +1077,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1074,7 +1091,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1088,7 +1105,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -1117,7 +1134,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
familyTree: added more text labels to nodes
</commit_message>
<xml_diff>
--- a/database/database.xlsx
+++ b/database/database.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="64">
   <si>
     <t>name</t>
   </si>
@@ -540,7 +540,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -628,7 +628,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -919,7 +919,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="C8" sqref="C8:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1073,6 +1073,9 @@
       <c r="A8" t="s">
         <v>44</v>
       </c>
+      <c r="E8" t="s">
+        <v>47</v>
+      </c>
       <c r="F8" t="s">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
sidebarFamily: added grid with family stats
</commit_message>
<xml_diff>
--- a/database/database.xlsx
+++ b/database/database.xlsx
@@ -628,7 +628,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -919,7 +919,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:C10"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
starting to display status as phenotype + genotype
</commit_message>
<xml_diff>
--- a/database/database.xlsx
+++ b/database/database.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="74">
   <si>
     <t>name</t>
   </si>
@@ -213,6 +213,36 @@
   </si>
   <si>
     <t>comments</t>
+  </si>
+  <si>
+    <t>phenotype</t>
+  </si>
+  <si>
+    <t>genotype</t>
+  </si>
+  <si>
+    <t>phenotypic-manifestation</t>
+  </si>
+  <si>
+    <t>mutation-carrier</t>
+  </si>
+  <si>
+    <t>no-mutation-carrier</t>
+  </si>
+  <si>
+    <t>not-genotyped</t>
+  </si>
+  <si>
+    <t>no-phenotypic-manifestation</t>
+  </si>
+  <si>
+    <t>sudden-cardiac-death</t>
+  </si>
+  <si>
+    <t>death-from-other-causes</t>
+  </si>
+  <si>
+    <t>ressucitated-scd-or-vf</t>
   </si>
 </sst>
 </file>
@@ -261,8 +291,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -270,9 +302,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -916,10 +950,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -930,9 +964,11 @@
     <col min="7" max="7" width="15.5" customWidth="1"/>
     <col min="8" max="8" width="16.1640625" customWidth="1"/>
     <col min="10" max="10" width="21.83203125" customWidth="1"/>
+    <col min="11" max="11" width="23.6640625" customWidth="1"/>
+    <col min="12" max="12" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -963,8 +999,14 @@
       <c r="J1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -980,8 +1022,14 @@
       <c r="I2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -997,8 +1045,14 @@
       <c r="I3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="K3" t="s">
+        <v>70</v>
+      </c>
+      <c r="L3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -1020,8 +1074,14 @@
       <c r="I4" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="K4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -1034,8 +1094,14 @@
       <c r="I5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="K5" t="s">
+        <v>73</v>
+      </c>
+      <c r="L5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>59</v>
       </c>
@@ -1051,8 +1117,14 @@
       <c r="I6" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="K6" t="s">
+        <v>66</v>
+      </c>
+      <c r="L6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1068,8 +1140,14 @@
       <c r="I7" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="K7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -1079,8 +1157,14 @@
       <c r="F8" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="K8" t="s">
+        <v>72</v>
+      </c>
+      <c r="L8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1093,8 +1177,14 @@
       <c r="I9" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="K9" t="s">
+        <v>66</v>
+      </c>
+      <c r="L9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1107,8 +1197,14 @@
       <c r="I10" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="K10" t="s">
+        <v>73</v>
+      </c>
+      <c r="L10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -1136,8 +1232,14 @@
       <c r="I11" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="K11" t="s">
+        <v>66</v>
+      </c>
+      <c r="L11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -1164,6 +1266,12 @@
       </c>
       <c r="I12" t="s">
         <v>57</v>
+      </c>
+      <c r="K12" t="s">
+        <v>71</v>
+      </c>
+      <c r="L12" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
display of patient's status as phenotype + genotype is done
</commit_message>
<xml_diff>
--- a/database/database.xlsx
+++ b/database/database.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="68">
   <si>
     <t>name</t>
   </si>
@@ -77,9 +77,6 @@
     <t>nhc</t>
   </si>
   <si>
-    <t>status</t>
-  </si>
-  <si>
     <t>dob</t>
   </si>
   <si>
@@ -167,9 +164,6 @@
     <t>none</t>
   </si>
   <si>
-    <t>sin-manifestacion-fenotipica</t>
-  </si>
-  <si>
     <t>diagnosed</t>
   </si>
   <si>
@@ -185,12 +179,6 @@
     <t>Suddent cardiac death</t>
   </si>
   <si>
-    <t>muerte-subita</t>
-  </si>
-  <si>
-    <t>portador-mutacion-responsable</t>
-  </si>
-  <si>
     <t>probando</t>
   </si>
   <si>
@@ -204,12 +192,6 @@
   </si>
   <si>
     <t>FJSL young brother</t>
-  </si>
-  <si>
-    <t>muerte-por-otras-causas</t>
-  </si>
-  <si>
-    <t>manifestacion-responsable</t>
   </si>
   <si>
     <t>comments</t>
@@ -291,8 +273,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -302,11 +290,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -574,7 +568,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -608,10 +602,10 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -699,243 +693,243 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" t="s">
         <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2" t="s">
-        <v>25</v>
       </c>
       <c r="G2" t="s">
         <v>5</v>
       </c>
       <c r="H2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G3" t="s">
         <v>5</v>
       </c>
       <c r="H3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
         <v>26</v>
-      </c>
-      <c r="B4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" t="s">
-        <v>27</v>
       </c>
       <c r="G4" t="s">
         <v>5</v>
       </c>
       <c r="H4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5" t="s">
         <v>5</v>
       </c>
       <c r="H5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
         <v>24</v>
-      </c>
-      <c r="E6" t="s">
-        <v>25</v>
       </c>
       <c r="G6" t="s">
         <v>5</v>
       </c>
       <c r="H6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
         <v>24</v>
-      </c>
-      <c r="E7" t="s">
-        <v>25</v>
       </c>
       <c r="G7" t="s">
         <v>5</v>
       </c>
       <c r="H7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" t="s">
         <v>44</v>
       </c>
-      <c r="B8" t="s">
-        <v>45</v>
-      </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
         <v>26</v>
-      </c>
-      <c r="E8" t="s">
-        <v>27</v>
       </c>
       <c r="G8" t="s">
         <v>5</v>
       </c>
       <c r="H8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G9" t="s">
         <v>7</v>
       </c>
       <c r="H9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" t="s">
         <v>29</v>
-      </c>
-      <c r="B10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" t="s">
-        <v>30</v>
       </c>
       <c r="G10" t="s">
         <v>7</v>
       </c>
       <c r="H10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G11" t="s">
         <v>7</v>
       </c>
       <c r="H11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G12" t="s">
         <v>7</v>
       </c>
       <c r="H12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -950,10 +944,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -961,14 +955,14 @@
     <col min="4" max="4" width="23.33203125" customWidth="1"/>
     <col min="5" max="5" width="20.83203125" customWidth="1"/>
     <col min="6" max="6" width="35.83203125" customWidth="1"/>
-    <col min="7" max="7" width="15.5" customWidth="1"/>
+    <col min="7" max="7" width="24.6640625" customWidth="1"/>
     <col min="8" max="8" width="16.1640625" customWidth="1"/>
     <col min="10" max="10" width="21.83203125" customWidth="1"/>
     <col min="11" max="11" width="23.6640625" customWidth="1"/>
     <col min="12" max="12" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -976,237 +970,207 @@
         <v>17</v>
       </c>
       <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>22</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
         <v>23</v>
-      </c>
-      <c r="I1" t="s">
-        <v>56</v>
-      </c>
-      <c r="J1" t="s">
-        <v>63</v>
-      </c>
-      <c r="K1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" t="s">
-        <v>24</v>
       </c>
       <c r="C2" s="1">
         <v>13516</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" t="s">
-        <v>57</v>
-      </c>
-      <c r="K2" t="s">
-        <v>66</v>
-      </c>
-      <c r="L2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+        <v>60</v>
+      </c>
+      <c r="G2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1">
         <v>15342</v>
       </c>
       <c r="E3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F3" t="s">
-        <v>61</v>
-      </c>
-      <c r="I3" t="s">
-        <v>57</v>
-      </c>
-      <c r="K3" t="s">
-        <v>70</v>
-      </c>
-      <c r="L3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+        <v>64</v>
+      </c>
+      <c r="G3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="1">
         <v>25569</v>
       </c>
       <c r="E4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" t="s">
+        <v>63</v>
+      </c>
+      <c r="H4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G5" t="s">
         <v>62</v>
       </c>
-      <c r="G4" t="s">
-        <v>49</v>
-      </c>
-      <c r="H4" t="s">
-        <v>50</v>
-      </c>
-      <c r="I4" t="s">
-        <v>58</v>
-      </c>
-      <c r="K4" t="s">
-        <v>71</v>
-      </c>
-      <c r="L4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" t="s">
-        <v>48</v>
-      </c>
-      <c r="I5" t="s">
-        <v>57</v>
-      </c>
-      <c r="K5" t="s">
-        <v>73</v>
-      </c>
-      <c r="L5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="J5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C6" s="1">
         <v>28856</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F6" t="s">
-        <v>48</v>
-      </c>
-      <c r="I6" t="s">
-        <v>57</v>
-      </c>
-      <c r="K6" t="s">
-        <v>66</v>
-      </c>
-      <c r="L6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+        <v>60</v>
+      </c>
+      <c r="G6" t="s">
+        <v>63</v>
+      </c>
+      <c r="J6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1">
         <v>24473</v>
       </c>
       <c r="E7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F7" t="s">
-        <v>48</v>
-      </c>
-      <c r="I7" t="s">
-        <v>57</v>
-      </c>
-      <c r="K7" t="s">
+        <v>60</v>
+      </c>
+      <c r="G7" t="s">
+        <v>61</v>
+      </c>
+      <c r="J7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" t="s">
         <v>66</v>
       </c>
-      <c r="L7" t="s">
+      <c r="G8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G9" t="s">
+        <v>63</v>
+      </c>
+      <c r="J9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" t="s">
-        <v>47</v>
-      </c>
-      <c r="F8" t="s">
-        <v>62</v>
-      </c>
-      <c r="K8" t="s">
-        <v>72</v>
-      </c>
-      <c r="L8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" t="s">
+      <c r="G10" t="s">
+        <v>61</v>
+      </c>
+      <c r="J10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
         <v>30</v>
-      </c>
-      <c r="E9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" t="s">
-        <v>48</v>
-      </c>
-      <c r="I9" t="s">
-        <v>57</v>
-      </c>
-      <c r="K9" t="s">
-        <v>66</v>
-      </c>
-      <c r="L9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" t="s">
-        <v>48</v>
-      </c>
-      <c r="I10" t="s">
-        <v>57</v>
-      </c>
-      <c r="K10" t="s">
-        <v>73</v>
-      </c>
-      <c r="L10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" t="s">
-        <v>31</v>
       </c>
       <c r="B11">
         <v>446093</v>
@@ -1215,33 +1179,30 @@
         <v>34335</v>
       </c>
       <c r="D11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F11" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" t="s">
+        <v>63</v>
+      </c>
+      <c r="H11" t="s">
+        <v>47</v>
+      </c>
+      <c r="I11" t="s">
+        <v>48</v>
+      </c>
+      <c r="J11" t="s">
         <v>54</v>
       </c>
-      <c r="G11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H11" t="s">
-        <v>50</v>
-      </c>
-      <c r="I11" t="s">
-        <v>58</v>
-      </c>
-      <c r="K11" t="s">
-        <v>66</v>
-      </c>
-      <c r="L11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12">
         <v>490754</v>
@@ -1250,28 +1211,25 @@
         <v>35796</v>
       </c>
       <c r="D12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" t="s">
         <v>47</v>
       </c>
-      <c r="F12" t="s">
-        <v>55</v>
-      </c>
-      <c r="G12" t="s">
-        <v>49</v>
-      </c>
-      <c r="H12" t="s">
-        <v>50</v>
-      </c>
       <c r="I12" t="s">
-        <v>57</v>
-      </c>
-      <c r="K12" t="s">
-        <v>71</v>
-      </c>
-      <c r="L12" t="s">
-        <v>67</v>
+        <v>48</v>
+      </c>
+      <c r="J12" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed "married_with" field from patients
</commit_message>
<xml_diff>
--- a/database/database.xlsx
+++ b/database/database.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2420" yWindow="640" windowWidth="28800" windowHeight="16920" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="2420" yWindow="640" windowWidth="28800" windowHeight="16920" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Family" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="67">
   <si>
     <t>name</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>mother</t>
-  </si>
-  <si>
-    <t>married_with</t>
   </si>
   <si>
     <t>family_id</t>
@@ -568,7 +565,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -602,10 +599,10 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -653,10 +650,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -665,7 +662,7 @@
     <col min="6" max="6" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -687,249 +684,228 @@
       <c r="G1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
         <v>23</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>32</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>41</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
         <v>24</v>
       </c>
-      <c r="G2" t="s">
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
         <v>5</v>
       </c>
-      <c r="H2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
+      <c r="G4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" t="s">
         <v>24</v>
       </c>
-      <c r="B3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" t="s">
         <v>5</v>
       </c>
-      <c r="H3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="G8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
         <v>41</v>
       </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="F10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
         <v>41</v>
       </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" t="s">
         <v>27</v>
       </c>
-      <c r="B7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="F11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
         <v>41</v>
       </c>
-      <c r="D7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" t="s">
-        <v>5</v>
-      </c>
-      <c r="H7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="D12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" t="s">
         <v>44</v>
-      </c>
-      <c r="C8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10" t="s">
-        <v>7</v>
-      </c>
-      <c r="H10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" t="s">
-        <v>28</v>
-      </c>
-      <c r="G11" t="s">
-        <v>7</v>
-      </c>
-      <c r="H11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" t="s">
-        <v>28</v>
-      </c>
-      <c r="G12" t="s">
-        <v>7</v>
-      </c>
-      <c r="H12" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -946,7 +922,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -967,210 +943,210 @@
         <v>10</v>
       </c>
       <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G1" t="s">
-        <v>59</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>21</v>
       </c>
-      <c r="I1" t="s">
-        <v>22</v>
-      </c>
       <c r="J1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="1">
         <v>13516</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" t="s">
         <v>60</v>
       </c>
-      <c r="G2" t="s">
-        <v>61</v>
-      </c>
       <c r="J2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="1">
         <v>15342</v>
       </c>
       <c r="E3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="1">
         <v>25569</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I4" t="s">
         <v>47</v>
       </c>
-      <c r="I4" t="s">
-        <v>48</v>
-      </c>
       <c r="J4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" s="1">
         <v>28856</v>
       </c>
       <c r="E6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="1">
         <v>24473</v>
       </c>
       <c r="E7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F7" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" t="s">
         <v>60</v>
       </c>
-      <c r="G7" t="s">
-        <v>61</v>
-      </c>
       <c r="J7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11">
         <v>446093</v>
@@ -1179,30 +1155,30 @@
         <v>34335</v>
       </c>
       <c r="D11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" t="s">
         <v>50</v>
       </c>
-      <c r="E11" t="s">
-        <v>51</v>
-      </c>
       <c r="F11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H11" t="s">
+        <v>46</v>
+      </c>
+      <c r="I11" t="s">
         <v>47</v>
       </c>
-      <c r="I11" t="s">
-        <v>48</v>
-      </c>
       <c r="J11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12">
         <v>490754</v>
@@ -1211,25 +1187,25 @@
         <v>35796</v>
       </c>
       <c r="D12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" t="s">
+        <v>64</v>
+      </c>
+      <c r="G12" t="s">
+        <v>60</v>
+      </c>
+      <c r="H12" t="s">
         <v>46</v>
       </c>
-      <c r="F12" t="s">
-        <v>65</v>
-      </c>
-      <c r="G12" t="s">
-        <v>61</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>47</v>
       </c>
-      <c r="I12" t="s">
-        <v>48</v>
-      </c>
       <c r="J12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
siebarFamily: redesign of cardFamily, starting to be able to edit diagnosis and mutations of a family (TODO: finishing the display of family statistics)
</commit_message>
<xml_diff>
--- a/database/database.xlsx
+++ b/database/database.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2420" yWindow="640" windowWidth="28800" windowHeight="16920" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2420" yWindow="640" windowWidth="28800" windowHeight="16920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Family" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="67">
   <si>
     <t>name</t>
   </si>
@@ -83,12 +83,6 @@
     <t>mutations</t>
   </si>
   <si>
-    <t>diagnostic_status</t>
-  </si>
-  <si>
-    <t>diagnostic</t>
-  </si>
-  <si>
     <t>upf_00201</t>
   </si>
   <si>
@@ -222,6 +216,12 @@
   </si>
   <si>
     <t>ressucitated-scd-or-vf</t>
+  </si>
+  <si>
+    <t>diagnosis</t>
+  </si>
+  <si>
+    <t>diagnosis_status</t>
   </si>
 </sst>
 </file>
@@ -270,8 +270,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -287,17 +289,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -573,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -586,9 +590,10 @@
     <col min="3" max="3" width="82.6640625" customWidth="1"/>
     <col min="4" max="4" width="32.6640625" customWidth="1"/>
     <col min="5" max="5" width="32" customWidth="1"/>
+    <col min="6" max="6" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -602,10 +607,13 @@
         <v>18</v>
       </c>
       <c r="E1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>65</v>
+      </c>
+      <c r="F1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -616,7 +624,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -627,7 +635,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -640,6 +648,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -652,7 +661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -687,225 +696,225 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
       </c>
       <c r="G3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
         <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F5" t="s">
         <v>5</v>
       </c>
       <c r="G5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F6" t="s">
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F7" t="s">
         <v>5</v>
       </c>
       <c r="G7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F8" t="s">
         <v>5</v>
       </c>
       <c r="G8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F9" t="s">
         <v>7</v>
       </c>
       <c r="G9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F10" t="s">
         <v>7</v>
       </c>
       <c r="G10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F11" t="s">
         <v>7</v>
       </c>
       <c r="G11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" t="s">
         <v>39</v>
       </c>
-      <c r="C12" t="s">
-        <v>41</v>
-      </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F12" t="s">
         <v>7</v>
       </c>
       <c r="G12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -923,7 +932,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -955,198 +964,198 @@
         <v>18</v>
       </c>
       <c r="F1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H1" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="I1" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="J1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C2" s="1">
         <v>13516</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1">
         <v>15342</v>
       </c>
       <c r="E3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1">
         <v>25569</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C6" s="1">
         <v>28856</v>
       </c>
       <c r="E6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C7" s="1">
         <v>24473</v>
       </c>
       <c r="E7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B11">
         <v>446093</v>
@@ -1155,30 +1164,30 @@
         <v>34335</v>
       </c>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B12">
         <v>490754</v>
@@ -1187,25 +1196,25 @@
         <v>35796</v>
       </c>
       <c r="D12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H12" t="s">
+        <v>44</v>
+      </c>
+      <c r="I12" t="s">
         <v>45</v>
       </c>
-      <c r="F12" t="s">
-        <v>64</v>
-      </c>
-      <c r="G12" t="s">
-        <v>60</v>
-      </c>
-      <c r="H12" t="s">
-        <v>46</v>
-      </c>
-      <c r="I12" t="s">
-        <v>47</v>
-      </c>
       <c r="J12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
restyling of cardFamilyWidgetStatistics + textFieldEditable
</commit_message>
<xml_diff>
--- a/database/database.xlsx
+++ b/database/database.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2420" yWindow="640" windowWidth="28800" windowHeight="16920" tabRatio="500"/>
+    <workbookView xWindow="2420" yWindow="640" windowWidth="28800" windowHeight="16920" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Family" sheetId="1" r:id="rId1"/>
@@ -569,7 +569,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -579,7 +579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -662,7 +662,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="A8" sqref="A2:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -931,8 +931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -993,7 +993,7 @@
         <v>43</v>
       </c>
       <c r="F2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G2" t="s">
         <v>58</v>
@@ -1096,7 +1096,7 @@
         <v>43</v>
       </c>
       <c r="F7" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G7" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
sidebarFamily: now family's diagnosis and mutations can be edited (and exported alongside with the rest of the family's data) + corrected general bugs related to the dob of the patients
</commit_message>
<xml_diff>
--- a/database/database.xlsx
+++ b/database/database.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2420" yWindow="640" windowWidth="28800" windowHeight="16920" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="6100" yWindow="2400" windowWidth="28800" windowHeight="16920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Family" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="71">
   <si>
     <t>name</t>
   </si>
@@ -222,13 +222,25 @@
   </si>
   <si>
     <t>diagnosis_status</t>
+  </si>
+  <si>
+    <t>Diagnosis 1, Diagnosis 2 test</t>
+  </si>
+  <si>
+    <t>Diagnosis 2 TEST</t>
+  </si>
+  <si>
+    <t>Gene1 + mutation in Gene1, Gene2 + mutation in Gene2</t>
+  </si>
+  <si>
+    <t>Gene34 + mutation in Gene34, Gene29 + mutation in Gene29</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -252,6 +264,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -270,7 +289,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -284,24 +303,37 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -569,7 +601,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -577,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -590,10 +622,11 @@
     <col min="3" max="3" width="82.6640625" customWidth="1"/>
     <col min="4" max="4" width="32.6640625" customWidth="1"/>
     <col min="5" max="5" width="32" customWidth="1"/>
-    <col min="6" max="6" width="26.5" customWidth="1"/>
+    <col min="6" max="6" width="52" customWidth="1"/>
+    <col min="7" max="7" width="29.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -610,10 +643,13 @@
         <v>65</v>
       </c>
       <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -624,7 +660,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -634,8 +670,14 @@
       <c r="C3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="E3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -644,6 +686,12 @@
       </c>
       <c r="C4" t="s">
         <v>9</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -931,7 +979,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -942,6 +990,7 @@
     <col min="6" max="6" width="35.83203125" customWidth="1"/>
     <col min="7" max="7" width="24.6640625" customWidth="1"/>
     <col min="8" max="8" width="16.1640625" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
     <col min="10" max="10" width="21.83203125" customWidth="1"/>
     <col min="11" max="11" width="23.6640625" customWidth="1"/>
     <col min="12" max="12" width="18" customWidth="1"/>

</xml_diff>

<commit_message>
pagePatients, export data: now the exported excel has the necessary format to be imported to the database
</commit_message>
<xml_diff>
--- a/database/database.xlsx
+++ b/database/database.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6100" yWindow="2400" windowWidth="28800" windowHeight="16920" tabRatio="500"/>
+    <workbookView xWindow="6100" yWindow="2400" windowWidth="28800" windowHeight="16920" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Family" sheetId="1" r:id="rId1"/>
@@ -152,9 +152,6 @@
     <t>UPF</t>
   </si>
   <si>
-    <t>none</t>
-  </si>
-  <si>
     <t>diagnosed</t>
   </si>
   <si>
@@ -234,6 +231,9 @@
   </si>
   <si>
     <t>Gene34 + mutation in Gene34, Gene29 + mutation in Gene29</t>
+  </si>
+  <si>
+    <t>asymptomatic</t>
   </si>
 </sst>
 </file>
@@ -601,7 +601,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -611,7 +611,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
@@ -640,13 +640,13 @@
         <v>18</v>
       </c>
       <c r="E1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F1" t="s">
         <v>19</v>
       </c>
       <c r="G1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -671,10 +671,10 @@
         <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -688,10 +688,10 @@
         <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -818,10 +818,10 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" t="s">
         <v>52</v>
-      </c>
-      <c r="B6" t="s">
-        <v>53</v>
       </c>
       <c r="C6" t="s">
         <v>38</v>
@@ -979,8 +979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1013,22 +1013,22 @@
         <v>18</v>
       </c>
       <c r="F1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" t="s">
         <v>55</v>
       </c>
-      <c r="G1" t="s">
-        <v>56</v>
-      </c>
       <c r="H1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -1039,16 +1039,16 @@
         <v>13516</v>
       </c>
       <c r="E2" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="F2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1059,16 +1059,16 @@
         <v>15342</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="F3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1079,22 +1079,22 @@
         <v>25569</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" t="s">
         <v>44</v>
       </c>
-      <c r="I4" t="s">
-        <v>45</v>
-      </c>
       <c r="J4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1102,36 +1102,36 @@
         <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="F5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" s="1">
         <v>28856</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="F6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1142,16 +1142,16 @@
         <v>24473</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="F7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1159,13 +1159,13 @@
         <v>40</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="F8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1173,16 +1173,16 @@
         <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="F9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1190,16 +1190,16 @@
         <v>25</v>
       </c>
       <c r="E10" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="F10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1213,25 +1213,25 @@
         <v>34335</v>
       </c>
       <c r="D11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" t="s">
         <v>47</v>
       </c>
-      <c r="E11" t="s">
-        <v>48</v>
-      </c>
       <c r="F11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H11" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" t="s">
         <v>44</v>
       </c>
-      <c r="I11" t="s">
-        <v>45</v>
-      </c>
       <c r="J11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1245,25 +1245,25 @@
         <v>35796</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E12" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" t="s">
         <v>43</v>
       </c>
-      <c r="F12" t="s">
-        <v>62</v>
-      </c>
-      <c r="G12" t="s">
-        <v>58</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>44</v>
       </c>
-      <c r="I12" t="s">
-        <v>45</v>
-      </c>
       <c r="J12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
use of Google Sheets API to read data of an existing drive's spreadsheet
</commit_message>
<xml_diff>
--- a/database/database.xlsx
+++ b/database/database.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6100" yWindow="2400" windowWidth="28800" windowHeight="16920" tabRatio="500"/>
+    <workbookView xWindow="6100" yWindow="2400" windowWidth="28800" windowHeight="16920" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Family" sheetId="1" r:id="rId1"/>
@@ -152,9 +152,6 @@
     <t>UPF</t>
   </si>
   <si>
-    <t>none</t>
-  </si>
-  <si>
     <t>diagnosed</t>
   </si>
   <si>
@@ -234,6 +231,9 @@
   </si>
   <si>
     <t>Gene34 + mutation in Gene34, Gene29 + mutation in Gene29</t>
+  </si>
+  <si>
+    <t>asymptomatic</t>
   </si>
 </sst>
 </file>
@@ -601,7 +601,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -611,7 +611,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
@@ -640,13 +640,13 @@
         <v>18</v>
       </c>
       <c r="E1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F1" t="s">
         <v>19</v>
       </c>
       <c r="G1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -671,10 +671,10 @@
         <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -688,10 +688,10 @@
         <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -818,10 +818,10 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" t="s">
         <v>52</v>
-      </c>
-      <c r="B6" t="s">
-        <v>53</v>
       </c>
       <c r="C6" t="s">
         <v>38</v>
@@ -979,8 +979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1013,22 +1013,22 @@
         <v>18</v>
       </c>
       <c r="F1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" t="s">
         <v>55</v>
       </c>
-      <c r="G1" t="s">
-        <v>56</v>
-      </c>
       <c r="H1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -1039,16 +1039,16 @@
         <v>13516</v>
       </c>
       <c r="E2" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="F2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1059,16 +1059,16 @@
         <v>15342</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="F3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1079,22 +1079,22 @@
         <v>25569</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" t="s">
         <v>44</v>
       </c>
-      <c r="I4" t="s">
-        <v>45</v>
-      </c>
       <c r="J4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1102,36 +1102,36 @@
         <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="F5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" s="1">
         <v>28856</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="F6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1142,16 +1142,16 @@
         <v>24473</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="F7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1159,13 +1159,13 @@
         <v>40</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="F8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1173,16 +1173,16 @@
         <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="F9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1190,16 +1190,16 @@
         <v>25</v>
       </c>
       <c r="E10" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="F10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1213,25 +1213,25 @@
         <v>34335</v>
       </c>
       <c r="D11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" t="s">
         <v>47</v>
       </c>
-      <c r="E11" t="s">
-        <v>48</v>
-      </c>
       <c r="F11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H11" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" t="s">
         <v>44</v>
       </c>
-      <c r="I11" t="s">
-        <v>45</v>
-      </c>
       <c r="J11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1245,25 +1245,25 @@
         <v>35796</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E12" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" t="s">
         <v>43</v>
       </c>
-      <c r="F12" t="s">
-        <v>62</v>
-      </c>
-      <c r="G12" t="s">
-        <v>58</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>44</v>
       </c>
-      <c r="I12" t="s">
-        <v>45</v>
-      </c>
       <c r="J12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>